<commit_message>
Update Agenda PDF and XLSX (26.06.2017)
</commit_message>
<xml_diff>
--- a/src/downloads/ui5con_2017_agenda.xlsx
+++ b/src/downloads/ui5con_2017_agenda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d068664\Documents\20170620 UI5Con\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d068664\WebstormProjects\gh-pages-openui5\ui5con\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Details" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agenda UI5con@SAP'!$A$1:$O$113</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agenda UI5con@SAP'!$A$1:$O$114</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Details!$A$1:$G$58</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Details!$1:$1</definedName>
   </definedNames>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="217">
   <si>
     <r>
       <rPr>
@@ -114,9 +114,6 @@
     <t>Jan Zaruba, Tomas Krejci</t>
   </si>
   <si>
-    <t>17:10 - 18:10</t>
-  </si>
-  <si>
     <t>Frederic Berg</t>
   </si>
   <si>
@@ -549,9 +546,6 @@
     <t>Session</t>
   </si>
   <si>
-    <t>All the news around UI5.</t>
-  </si>
-  <si>
     <t>Key Note</t>
   </si>
   <si>
@@ -603,9 +597,6 @@
     <t>We will present newly released and upcoming controls which we have developed in Brno Suite Controls team. We will have prototypes and demos ready for the upcoming controls and demo apps for released controls. We’ll be happy to answer any questions regarding implementation of our controls in your apps.</t>
   </si>
   <si>
-    <t>Session Description: In this session we will write a custom component using OpenLayers v3 (http://www.openlayers.de) for showing a map. This map will be bound to a XMPPJsonPatchSyncModel (https://github.com/ManuelB/XMPPJSONPatchSyncModel) to make it possible to track other people in real time on the map.</t>
-  </si>
-  <si>
     <t>In our UI5 demo app, you'll learn to build an ice cream machine. We will show the demo app and a tutorial with a step-by-step explanation of how to build this app using various UI5 Controls.</t>
   </si>
   <si>
@@ -718,13 +709,25 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>17:20 - 18:20</t>
+  </si>
+  <si>
+    <t>Last updated: 26.06.2017 14:45</t>
+  </si>
+  <si>
+    <t>SAPUI5 is evolving and thus best practices or recommended controls change over time. In this session, you'll get an update on the new supportability tool, the new DemoKit, new and updated controls, news in the framework like our plans towards OData V4 and improved Smart Controls. Finally we'll share some insights into more radical renovation activities that will come early in 2018.</t>
+  </si>
+  <si>
+    <t>In this session we will use a custom component (https://github.com/ManuelB/openui5-ol/) that wraps the OpenLayers v3 API (http://www.openlayers.de) for showing a map. This map will be bound to a XMPPJsonPatchSyncModel (https://github.com/ManuelB/XMPPJSONPatchSyncModel) to make it possible to track other people in real time on the map.You should pre-install the following software on your notebook:  git  Your favorite IDE  ejabbered (a public server will be running on the speaker notebook)  A webserver e.g. (python -m SimpleHTTPServer 8000)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -808,6 +811,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFF26A36"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -896,7 +906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -936,6 +946,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,9 +1278,7 @@
   </sheetPr>
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="A58" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1350,11 +1371,11 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -1442,11 +1463,11 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
@@ -1463,7 +1484,7 @@
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O5" s="6">
         <v>0.40277777777777801</v>
@@ -1488,11 +1509,11 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -1534,11 +1555,11 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1547,11 +1568,11 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="10" t="s">
@@ -1739,7 +1760,7 @@
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O11" s="6">
         <v>0.42361111111111099</v>
@@ -1785,7 +1806,7 @@
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O12" s="6">
         <v>0.42708333333333398</v>
@@ -1810,11 +1831,11 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1823,15 +1844,15 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O13" s="6">
         <v>0.43055555555555602</v>
@@ -1856,11 +1877,11 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1869,11 +1890,11 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="10" t="s">
@@ -1994,24 +2015,24 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="1"/>
       <c r="J17" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="10" t="s">
@@ -2107,7 +2128,7 @@
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O19" s="6">
         <v>0.45138888888889001</v>
@@ -2153,7 +2174,7 @@
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O20" s="6">
         <v>0.45486111111111199</v>
@@ -2199,7 +2220,7 @@
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O21" s="6">
         <v>0.45833333333333398</v>
@@ -2270,11 +2291,11 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="10" t="s">
@@ -2283,11 +2304,11 @@
       <c r="H23" s="18"/>
       <c r="I23" s="1"/>
       <c r="J23" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="10" t="s">
@@ -2316,11 +2337,11 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="10" t="s">
@@ -2329,11 +2350,11 @@
       <c r="H24" s="18"/>
       <c r="I24" s="1"/>
       <c r="J24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="10" t="s">
@@ -2454,24 +2475,24 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="1"/>
       <c r="J27" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M27" s="1"/>
       <c r="N27" s="10" t="s">
@@ -2508,7 +2529,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="1"/>
@@ -2646,7 +2667,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="1"/>
@@ -2659,7 +2680,7 @@
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O31" s="6">
         <v>0.49305555555555702</v>
@@ -2705,7 +2726,7 @@
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O32" s="6">
         <v>0.49652777777777901</v>
@@ -2730,11 +2751,11 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2743,15 +2764,15 @@
       <c r="H33" s="18"/>
       <c r="I33" s="1"/>
       <c r="J33" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O33" s="6">
         <v>0.500000000000001</v>
@@ -2776,11 +2797,11 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="10" t="s">
@@ -2789,11 +2810,11 @@
       <c r="H34" s="18"/>
       <c r="I34" s="1"/>
       <c r="J34" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M34" s="1"/>
       <c r="N34" s="10" t="s">
@@ -2914,11 +2935,11 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="10" t="s">
@@ -3010,7 +3031,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="10" t="s">
@@ -3056,7 +3077,7 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="10" t="s">
@@ -3106,7 +3127,7 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="1"/>
@@ -3152,7 +3173,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="1"/>
@@ -3190,7 +3211,7 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -3211,7 +3232,7 @@
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O43" s="6">
         <v>0.53472222222222399</v>
@@ -3236,7 +3257,7 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
@@ -3257,7 +3278,7 @@
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O44" s="6">
         <v>0.53819444444444597</v>
@@ -3295,15 +3316,15 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O45" s="6">
         <v>0.54166666666666796</v>
@@ -3562,7 +3583,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -3571,11 +3592,11 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K51" s="1"/>
       <c r="L51" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M51" s="1"/>
       <c r="N51" s="10" t="s">
@@ -3617,11 +3638,11 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K52" s="1"/>
       <c r="L52" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M52" s="1"/>
       <c r="N52" s="10" t="s">
@@ -3658,7 +3679,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="1"/>
@@ -3742,7 +3763,7 @@
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="10" t="s">
@@ -3755,15 +3776,15 @@
       <c r="H55" s="18"/>
       <c r="I55" s="1"/>
       <c r="J55" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K55" s="1"/>
       <c r="L55" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O55" s="6">
         <v>0.57638888888889095</v>
@@ -3809,7 +3830,7 @@
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O56" s="6">
         <v>0.57986111111111305</v>
@@ -3834,11 +3855,11 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="10" t="s">
@@ -3855,7 +3876,7 @@
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O57" s="6">
         <v>0.58333333333333504</v>
@@ -3880,11 +3901,11 @@
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="10" t="s">
@@ -4018,11 +4039,11 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="10" t="s">
@@ -4031,11 +4052,11 @@
       <c r="H61" s="18"/>
       <c r="I61" s="1"/>
       <c r="J61" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K61" s="1"/>
       <c r="L61" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M61" s="1"/>
       <c r="N61" s="10" t="s">
@@ -4077,11 +4098,11 @@
       <c r="H62" s="18"/>
       <c r="I62" s="1"/>
       <c r="J62" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M62" s="1"/>
       <c r="N62" s="10" t="s">
@@ -4110,15 +4131,15 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="1"/>
@@ -4156,15 +4177,15 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H64" s="18"/>
       <c r="I64" s="1"/>
@@ -4215,11 +4236,11 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K65" s="1"/>
       <c r="L65" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M65" s="1"/>
       <c r="N65" s="10" t="s">
@@ -4294,15 +4315,15 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="1"/>
@@ -4315,7 +4336,7 @@
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O67" s="6">
         <v>0.61805555555555802</v>
@@ -4361,7 +4382,7 @@
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O68" s="6">
         <v>0.62152777777778001</v>
@@ -4386,11 +4407,11 @@
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="10" t="s">
@@ -4407,7 +4428,7 @@
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O69" s="6">
         <v>0.625000000000003</v>
@@ -4432,11 +4453,11 @@
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="10" t="s">
@@ -4491,11 +4512,11 @@
       <c r="H71" s="18"/>
       <c r="I71" s="1"/>
       <c r="J71" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M71" s="1"/>
       <c r="N71" s="10" t="s">
@@ -4537,11 +4558,11 @@
       <c r="H72" s="18"/>
       <c r="I72" s="1"/>
       <c r="J72" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M72" s="1"/>
       <c r="N72" s="10" t="s">
@@ -4570,11 +4591,11 @@
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="10" t="s">
@@ -4662,11 +4683,11 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="10" t="s">
@@ -4675,11 +4696,11 @@
       <c r="H75" s="18"/>
       <c r="I75" s="1"/>
       <c r="J75" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K75" s="1"/>
       <c r="L75" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M75" s="1"/>
       <c r="N75" s="10" t="s">
@@ -4708,11 +4729,11 @@
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="10" t="s">
@@ -4762,7 +4783,7 @@
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="1"/>
@@ -4808,7 +4829,7 @@
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H78" s="18"/>
       <c r="I78" s="1"/>
@@ -4846,11 +4867,11 @@
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
@@ -4867,7 +4888,7 @@
       </c>
       <c r="M79" s="1"/>
       <c r="N79" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O79" s="6">
         <v>0.65972222222222499</v>
@@ -4913,7 +4934,7 @@
       </c>
       <c r="M80" s="1"/>
       <c r="N80" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O80" s="6">
         <v>0.66319444444444697</v>
@@ -4946,20 +4967,20 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="1"/>
       <c r="J81" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K81" s="1"/>
       <c r="L81" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M81" s="1"/>
       <c r="N81" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O81" s="6">
         <v>0.66666666666666996</v>
@@ -4997,11 +5018,11 @@
       <c r="H82" s="18"/>
       <c r="I82" s="1"/>
       <c r="J82" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K82" s="1"/>
       <c r="L82" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M82" s="1"/>
       <c r="N82" s="10" t="s">
@@ -5122,11 +5143,11 @@
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="10" t="s">
@@ -5135,11 +5156,11 @@
       <c r="H85" s="18"/>
       <c r="I85" s="1"/>
       <c r="J85" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K85" s="1"/>
       <c r="L85" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M85" s="1"/>
       <c r="N85" s="10" t="s">
@@ -5168,11 +5189,11 @@
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="10" t="s">
@@ -5306,11 +5327,11 @@
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="10" t="s">
@@ -5406,20 +5427,20 @@
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H91" s="18"/>
       <c r="I91" s="1"/>
       <c r="J91" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K91" s="1"/>
       <c r="L91" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M91" s="1"/>
       <c r="N91" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O91" s="6">
         <v>0.70138888888889195</v>
@@ -5452,20 +5473,20 @@
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H92" s="18"/>
       <c r="I92" s="1"/>
       <c r="J92" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K92" s="1"/>
       <c r="L92" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M92" s="1"/>
       <c r="N92" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O92" s="6">
         <v>0.70486111111111505</v>
@@ -5528,7 +5549,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>0.71180555555555902</v>
       </c>
@@ -5578,16 +5599,14 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F95" s="1"/>
-      <c r="G95" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="G95" s="1"/>
       <c r="H95" s="17"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1" t="s">
@@ -5622,16 +5641,14 @@
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F96" s="1"/>
-      <c r="G96" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="G96" s="1"/>
       <c r="H96" s="18"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1" t="s">
@@ -5673,8 +5690,8 @@
         <v>10</v>
       </c>
       <c r="F97" s="1"/>
-      <c r="G97" s="10" t="s">
-        <v>10</v>
+      <c r="G97" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="H97" s="18"/>
       <c r="I97" s="1"/>
@@ -5746,11 +5763,11 @@
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="10" t="s">
@@ -5826,11 +5843,11 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="10" t="s">
@@ -5865,11 +5882,11 @@
         <v>0.73958333333333703</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="10" t="s">
@@ -5949,15 +5966,15 @@
         <v>0.750000000000004</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="1"/>
@@ -5972,7 +5989,7 @@
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
     </row>
-    <row r="106" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>0.75347222222222598</v>
       </c>
@@ -5984,8 +6001,8 @@
         <v>10</v>
       </c>
       <c r="F106" s="1"/>
-      <c r="G106" s="11" t="s">
-        <v>14</v>
+      <c r="G106" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="1"/>
@@ -6012,7 +6029,9 @@
         <v>12</v>
       </c>
       <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
+      <c r="G107" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
@@ -6038,7 +6057,9 @@
         <v>11</v>
       </c>
       <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
+      <c r="G108" s="11" t="s">
+        <v>213</v>
+      </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
@@ -6154,11 +6175,18 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
-      <c r="O113" s="6"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="6"/>
-      <c r="O114" s="6"/>
+      <c r="A114" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="B114" s="23"/>
+      <c r="C114" s="19"/>
+      <c r="N114" s="20" t="str">
+        <f>A114</f>
+        <v>Last updated: 26.06.2017 14:45</v>
+      </c>
+      <c r="O114" s="21"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
@@ -6273,8 +6301,12 @@
       <c r="O142" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N114:O114"/>
+    <mergeCell ref="A114:C114"/>
+  </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="44" fitToWidth="2" orientation="portrait" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" fitToWidth="2" orientation="portrait" blackAndWhite="1" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="44" max="16383" man="1"/>
   </rowBreaks>
@@ -6291,8 +6323,8 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A19" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6308,25 +6340,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>153</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6337,13 +6369,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -6356,13 +6388,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -6378,19 +6410,19 @@
         <v>7</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F4" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>0.40972222222222227</v>
       </c>
@@ -6398,22 +6430,22 @@
         <v>0.4375</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>0.40972222222222227</v>
       </c>
@@ -6421,19 +6453,19 @@
         <v>0.4375</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6447,16 +6479,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -6470,16 +6502,16 @@
         <v>6</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6493,16 +6525,16 @@
         <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6513,19 +6545,19 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -6536,19 +6568,19 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -6559,19 +6591,19 @@
         <v>0.4861111111111111</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6585,16 +6617,16 @@
         <v>5</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6608,16 +6640,16 @@
         <v>6</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6631,16 +6663,16 @@
         <v>7</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6651,19 +6683,19 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6674,19 +6706,19 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6700,16 +6732,16 @@
         <v>5</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6723,19 +6755,19 @@
         <v>6</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>0.49305555555555558</v>
       </c>
@@ -6743,19 +6775,19 @@
         <v>0.53472222222222221</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6769,16 +6801,16 @@
         <v>7</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6789,19 +6821,19 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6812,19 +6844,19 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D23" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>107</v>
-      </c>
       <c r="F23" s="15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6838,16 +6870,16 @@
         <v>5</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -6861,16 +6893,16 @@
         <v>6</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6884,16 +6916,16 @@
         <v>7</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6904,19 +6936,19 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6927,19 +6959,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C28" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="G28" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6950,19 +6982,19 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6976,16 +7008,16 @@
         <v>5</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6999,16 +7031,16 @@
         <v>6</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7022,16 +7054,16 @@
         <v>7</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -7042,19 +7074,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -7065,19 +7097,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7091,16 +7123,16 @@
         <v>5</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7114,16 +7146,16 @@
         <v>6</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7134,19 +7166,19 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7157,19 +7189,19 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7180,19 +7212,19 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="C39" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G39" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7206,16 +7238,16 @@
         <v>7</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7226,19 +7258,19 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7249,19 +7281,19 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7275,16 +7307,16 @@
         <v>5</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7298,16 +7330,16 @@
         <v>6</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7318,19 +7350,19 @@
         <v>0.6875</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7341,19 +7373,19 @@
         <v>0.6875</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7364,19 +7396,19 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C47" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G47" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7390,16 +7422,16 @@
         <v>7</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7413,16 +7445,16 @@
         <v>5</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7436,16 +7468,16 @@
         <v>6</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7456,19 +7488,19 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7479,19 +7511,19 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7502,19 +7534,19 @@
         <v>0.75694444444444453</v>
       </c>
       <c r="C53" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G53" s="15" t="s">
         <v>167</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7525,19 +7557,19 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7548,19 +7580,19 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7571,19 +7603,19 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7594,19 +7626,19 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -7617,7 +7649,7 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="15" t="s">

</xml_diff>

<commit_message>
Update Hands-On Prerequisites, PDF and XLSX (27.06.2017)
</commit_message>
<xml_diff>
--- a/src/downloads/ui5con_2017_agenda.xlsx
+++ b/src/downloads/ui5con_2017_agenda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d068664\WebstormProjects\gh-pages-openui5\ui5con\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d068664\WebstormProjects\ui5con\src\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agenda UI5con@SAP'!$A$1:$O$114</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Details!$A$1:$G$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Details!$A$1:$G$57</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Details!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="219">
   <si>
     <r>
       <rPr>
@@ -153,9 +153,6 @@
     <t>16:00 - 17:00</t>
   </si>
   <si>
-    <t>16:20 - 17:00</t>
-  </si>
-  <si>
     <t>Christoph Laux</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Mateusz Skadorwa, Tomasz Wilk</t>
   </si>
   <si>
-    <t>15:30 - 16:10</t>
-  </si>
-  <si>
     <t>Integrate Feed Capabilities Using UI5 Controls</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
     <t>Building a companion conversational UI for a Fiori App</t>
   </si>
   <si>
-    <t>14:40 - 15:20</t>
-  </si>
-  <si>
     <t>Vered Constantin</t>
   </si>
   <si>
@@ -300,15 +291,9 @@
     <t>Michael Graf, Emanuele Ricci</t>
   </si>
   <si>
-    <t>13:50 - 14:30</t>
-  </si>
-  <si>
     <t>Stephan Heyne</t>
   </si>
   <si>
-    <t>Peter Muessig, Matthias Osswal</t>
-  </si>
-  <si>
     <t>The UI5 app to create UI5 apps</t>
   </si>
   <si>
@@ -348,9 +333,6 @@
     <t>Functional Programming for your UI5 App</t>
   </si>
   <si>
-    <t>13:00 - 13:40</t>
-  </si>
-  <si>
     <t>Helmut Tammen</t>
   </si>
   <si>
@@ -414,9 +396,6 @@
     <t>HP Seitz</t>
   </si>
   <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
     <t>Pia Kinkel, Bohdan Pukalskyi, Dominic Holzwarth</t>
   </si>
   <si>
@@ -459,9 +438,6 @@
     <t>Developer Clinic: UI5 Controls</t>
   </si>
   <si>
-    <t>10:20 - 11:00</t>
-  </si>
-  <si>
     <t>The OpenUI5 Developer Blog - Behind the Scenes</t>
   </si>
   <si>
@@ -489,9 +465,6 @@
     <t>Stefan Beck</t>
   </si>
   <si>
-    <t>09:40 - 10:20</t>
-  </si>
-  <si>
     <t>Pia Kinkel, Christoph Laux</t>
   </si>
   <si>
@@ -549,9 +522,6 @@
     <t>Key Note</t>
   </si>
   <si>
-    <t>Demo new upcoming features of UI5 regarding Metadata Driven Controls.Allow to manipulate the artifacts live in an editor and see the immediate result.Create custom control using a Fragment Control, add a Swagger service to the View and enhance the metadata.Drive the new custom control and other UI controls from the metadata.</t>
-  </si>
-  <si>
     <t>Imagine a world where development and business can understand each other without using lengthy code lines. Applying human-readable language you will have the possibility to enable everyone in your team, even your customers, to create business driven automated tests.Our solution will lead your agile workflow towards acceptance testing using OPA5 and Cucumber over Fiori stack which provide basis for behavior driven development.We are going to present a Cucumber and OPA5-based test automation framework where users write test scenarios adopting human-readable Gherkin language. Additionally, we will talk about the key test concepts of healthy test automation pyramids, appropriate placement of test levels, and misconcepts about TDD and BDD.</t>
   </si>
   <si>
@@ -651,9 +621,6 @@
     <t>Session Description: In this session I will discuss options how UI5 web apps can be used as a basis for apps beyond your typical office requirements. While SAP Fiori apps and Fiori LaunchPad are the basis for SAPs Digital Workplace of the future, there exist much more possibilities how the web can be the basis for your digitalization efforts. We are looking into WebAPIs, standards such as WebRTC and 3rd party extensions and how this can be applied in enterprise settings. Adding Cloud APIs into the mix, lots of demand for feature-rich apps can already be fulfilled leveraging the web.</t>
   </si>
   <si>
-    <t>Let`s build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind.</t>
-  </si>
-  <si>
     <t>Building a Conversational UI for the Fiori My Inbox app using API.AI. I will run through the code needed and do a live demo.</t>
   </si>
   <si>
@@ -672,9 +639,6 @@
     <t>Based on a public OpenUI5 boilerplate project (not published, yet) we want to share our experience and knowledge on how to setup and use a modern OpenUI5 app structure and build process by using Babel, Flow and Gulp (especially addressing non-SAP developers). Furthermore an overview of very useful best practices, does &amp; don'ts and quick enhancements (like new useful methods in the app Component and BaseController) that should speed up your development workflow and that keep the app maintainable and scalable.</t>
   </si>
   <si>
-    <t>Find out everything you need to know about the new version of SAP Fiori. Learn what makes Fiori 2.0 different and which are the new UI5 features empowering Fiori 2.0 experience.In this session we will show and tell how to develop your Fiori 2.0 app from scratch and even more - how to migrate your existing app to Fiori 2.0.</t>
-  </si>
-  <si>
     <t>Social media is ubiquitous, but a feed can also include system events or comments. UI5 provides a set of controls that support you in implementing feed capabilities for your application.</t>
   </si>
   <si>
@@ -690,9 +654,6 @@
     <t>What is SAP's new extensibility approach all about? Well, the key is flexibility. Partners and customers need to adapt the UIs of SAP apps, for example add, hide or rearrange fields. Sounds technical and complicated? SAPUI5 extensibility changes all that allowing upgrade-safe, modification-free, and role-based UI changes with intuitive and easy-to-use tools – even for non-developers.What's the strategy behind it, what are the benefits, and what's the roadmap? In this session you'll find out.</t>
   </si>
   <si>
-    <t>In this session, we will demonstrate how to get started on cloud foundry. We will see how to onboard onto the platform, install the necessary tools and deploy a UI5 application which makes use of platform services to persist its data.</t>
-  </si>
-  <si>
     <t>It all started with a Proof-of-Concept of a UI5 hybrid application for discrete object recognition on mobile devices. In the course of the PoC, research led to several experiments around the key words in the session title: from real-time Image manipulation via visual object recognition up to Augmented Reality flavors, all of that within the UI5 framework. I'd like to show the results of the experiments and evaluate their sustainability and production readiness.</t>
   </si>
   <si>
@@ -714,13 +675,58 @@
     <t>17:20 - 18:20</t>
   </si>
   <si>
-    <t>Last updated: 26.06.2017 14:45</t>
-  </si>
-  <si>
     <t>SAPUI5 is evolving and thus best practices or recommended controls change over time. In this session, you'll get an update on the new supportability tool, the new DemoKit, new and updated controls, news in the framework like our plans towards OData V4 and improved Smart Controls. Finally we'll share some insights into more radical renovation activities that will come early in 2018.</t>
   </si>
   <si>
     <t>In this session we will use a custom component (https://github.com/ManuelB/openui5-ol/) that wraps the OpenLayers v3 API (http://www.openlayers.de) for showing a map. This map will be bound to a XMPPJsonPatchSyncModel (https://github.com/ManuelB/XMPPJSONPatchSyncModel) to make it possible to track other people in real time on the map.You should pre-install the following software on your notebook:  git  Your favorite IDE  ejabbered (a public server will be running on the speaker notebook)  A webserver e.g. (python -m SimpleHTTPServer 8000)</t>
+  </si>
+  <si>
+    <t>10:50 - 11:30</t>
+  </si>
+  <si>
+    <t>11:40 - 12:20</t>
+  </si>
+  <si>
+    <t>12:30 - 13:10</t>
+  </si>
+  <si>
+    <t>14:00 - 14:40</t>
+  </si>
+  <si>
+    <t>Peter Muessig, Matthias Oßwald</t>
+  </si>
+  <si>
+    <t>14:50 - 15:30</t>
+  </si>
+  <si>
+    <t>15:40 - 16:20</t>
+  </si>
+  <si>
+    <t>16:30 - 17:10</t>
+  </si>
+  <si>
+    <t>17:20 - 18:00</t>
+  </si>
+  <si>
+    <t>11:20 - 12:00</t>
+  </si>
+  <si>
+    <t>17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Concepts of upcoming features of UI5 to ease creation of building blocks and connection of controls to Rest Service Metadata.</t>
+  </si>
+  <si>
+    <t>Find out everything you need to know about the new version of SAP Fiori. Learn what makes Fiori 2.0 different and which are the new UI5 features empowering Fiori 2.0 experience.In this session we will show and tell how to develop your Fiori 2.0 app from scratch and even more - how to migrate your existing app to Fiori 2.0.Prerequisites:You will work in SAP WebIDE, trial accounts are already created for you, so you do not need anything else than your laptop. In case of network issues, we would fall back to using nodejs, NPM and Git, so you should preferably have those installed.</t>
+  </si>
+  <si>
+    <t>In this session, we will demonstrate how to get started on cloud foundry. We will see how to onboard onto the platform, install the necessary tools and deploy a UI5 application which makes use of platform services to persist its data.Prerequisites:Please have Node.js installed on your laptop and your own hanatrial account ready.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind. Prerequisites:   - Laptop  - an SAP CP trial account </t>
+  </si>
+  <si>
+    <t>Last updated: 27.06.2017 14:55</t>
   </si>
 </sst>
 </file>
@@ -946,7 +952,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -959,6 +964,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1278,7 +1284,9 @@
   </sheetPr>
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:C114"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1371,11 +1379,11 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="9" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="9" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -1383,17 +1391,11 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="6">
         <v>0.39583333333333331</v>
       </c>
@@ -1411,7 +1413,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0.39930555555555558</v>
       </c>
@@ -1429,17 +1431,11 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="6">
         <v>0.39930555555555558</v>
       </c>
@@ -1475,17 +1471,6 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="9" t="s">
-        <v>146</v>
-      </c>
       <c r="O5" s="6">
         <v>0.40277777777777801</v>
       </c>
@@ -1509,11 +1494,11 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -1521,17 +1506,6 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O6" s="6">
         <v>0.40625</v>
       </c>
@@ -1555,11 +1529,11 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="9" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="9" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1567,17 +1541,6 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O7" s="6">
         <v>0.40972222222222199</v>
       </c>
@@ -1613,17 +1576,6 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O8" s="6">
         <v>0.41319444444444497</v>
       </c>
@@ -1659,17 +1611,6 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O9" s="6">
         <v>0.41666666666666702</v>
       </c>
@@ -1705,17 +1646,6 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O10" s="6">
         <v>0.42013888888888901</v>
       </c>
@@ -1751,17 +1681,6 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="10" t="s">
-        <v>140</v>
-      </c>
       <c r="O11" s="6">
         <v>0.42361111111111099</v>
       </c>
@@ -1779,7 +1698,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>0.42708333333333398</v>
       </c>
@@ -1797,17 +1716,6 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="11" t="s">
-        <v>139</v>
-      </c>
       <c r="O12" s="6">
         <v>0.42708333333333398</v>
       </c>
@@ -1831,11 +1739,11 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="10" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1843,17 +1751,6 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="M13" s="1"/>
-      <c r="N13" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="O13" s="6">
         <v>0.43055555555555602</v>
       </c>
@@ -1877,11 +1774,11 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1889,17 +1786,6 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O14" s="6">
         <v>0.43402777777777801</v>
       </c>
@@ -1935,15 +1821,13 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="10" t="s">
+      <c r="J15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="O15" s="6">
@@ -1981,15 +1865,13 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="10" t="s">
+      <c r="J16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="O16" s="6">
@@ -2015,28 +1897,28 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="9" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="9" t="s">
-        <v>131</v>
+      <c r="J17" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="9" t="s">
-        <v>130</v>
+      <c r="L17" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="10" t="s">
-        <v>10</v>
+      <c r="N17" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="O17" s="6">
         <v>0.44444444444444497</v>
@@ -2055,7 +1937,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>0.44791666666666702</v>
       </c>
@@ -2073,11 +1955,11 @@
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M18" s="1"/>
@@ -2119,16 +2001,16 @@
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="10" t="s">
-        <v>10</v>
+      <c r="J19" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" s="10" t="s">
-        <v>10</v>
+      <c r="L19" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="10" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="O19" s="6">
         <v>0.45138888888889001</v>
@@ -2147,7 +2029,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>0.45486111111111199</v>
       </c>
@@ -2173,8 +2055,8 @@
         <v>10</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="N20" s="11" t="s">
-        <v>129</v>
+      <c r="N20" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="O20" s="6">
         <v>0.45486111111111199</v>
@@ -2219,8 +2101,8 @@
         <v>10</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="9" t="s">
-        <v>128</v>
+      <c r="N21" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="O21" s="6">
         <v>0.45833333333333398</v>
@@ -2291,11 +2173,11 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="10" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="10" t="s">
@@ -2304,15 +2186,15 @@
       <c r="H23" s="18"/>
       <c r="I23" s="1"/>
       <c r="J23" s="10" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="10" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="10" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="O23" s="6">
         <v>0.46527777777777901</v>
@@ -2337,11 +2219,11 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="11" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="11" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="10" t="s">
@@ -2349,16 +2231,16 @@
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="11" t="s">
-        <v>123</v>
+      <c r="J24" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" s="11" t="s">
-        <v>123</v>
+      <c r="L24" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M24" s="1"/>
-      <c r="N24" s="10" t="s">
-        <v>10</v>
+      <c r="N24" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="O24" s="6">
         <v>0.468750000000001</v>
@@ -2395,16 +2277,16 @@
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1" t="s">
-        <v>10</v>
+      <c r="J25" s="10" t="s">
+        <v>129</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" s="1" t="s">
-        <v>10</v>
+      <c r="L25" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="M25" s="1"/>
-      <c r="N25" s="10" t="s">
-        <v>10</v>
+      <c r="N25" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="O25" s="6">
         <v>0.47222222222222299</v>
@@ -2441,12 +2323,12 @@
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1" t="s">
-        <v>10</v>
+      <c r="J26" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="1" t="s">
-        <v>10</v>
+      <c r="L26" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="10" t="s">
@@ -2475,24 +2357,24 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="10" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="9" t="s">
-        <v>119</v>
+      <c r="J27" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="L27" s="9" t="s">
-        <v>118</v>
+      <c r="L27" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M27" s="1"/>
       <c r="N27" s="10" t="s">
@@ -2529,15 +2411,15 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="10" t="s">
+      <c r="L28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M28" s="1"/>
@@ -2579,12 +2461,12 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="10" t="s">
-        <v>10</v>
+      <c r="J29" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="L29" s="10" t="s">
-        <v>10</v>
+      <c r="L29" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="10" t="s">
@@ -2667,7 +2549,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="9" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="1"/>
@@ -2680,7 +2562,7 @@
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="10" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="O31" s="6">
         <v>0.49305555555555702</v>
@@ -2726,7 +2608,7 @@
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="11" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="O32" s="6">
         <v>0.49652777777777901</v>
@@ -2751,11 +2633,11 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2764,15 +2646,15 @@
       <c r="H33" s="18"/>
       <c r="I33" s="1"/>
       <c r="J33" s="10" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="10" t="s">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="9" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="O33" s="6">
         <v>0.500000000000001</v>
@@ -2797,11 +2679,11 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="11" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="10" t="s">
@@ -2809,12 +2691,12 @@
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="11" t="s">
-        <v>108</v>
+      <c r="J34" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="L34" s="11" t="s">
-        <v>108</v>
+      <c r="L34" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M34" s="1"/>
       <c r="N34" s="10" t="s">
@@ -2855,12 +2737,12 @@
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1" t="s">
-        <v>10</v>
+      <c r="J35" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="K35" s="1"/>
-      <c r="L35" s="1" t="s">
-        <v>10</v>
+      <c r="L35" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="10" t="s">
@@ -2901,12 +2783,12 @@
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1" t="s">
-        <v>10</v>
+      <c r="J36" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" s="1" t="s">
-        <v>10</v>
+      <c r="L36" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="10" t="s">
@@ -2935,11 +2817,11 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="10" t="s">
@@ -2975,7 +2857,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>0.51736111111111205</v>
       </c>
@@ -3031,7 +2913,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="10" t="s">
@@ -3039,12 +2921,12 @@
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1" t="s">
-        <v>10</v>
+      <c r="J39" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="K39" s="1"/>
-      <c r="L39" s="1" t="s">
-        <v>10</v>
+      <c r="L39" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="10" t="s">
@@ -3077,7 +2959,7 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="10" t="s">
@@ -3085,11 +2967,11 @@
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K40" s="1"/>
-      <c r="L40" s="1" t="s">
+      <c r="L40" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M40" s="1"/>
@@ -3127,15 +3009,15 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1" t="s">
+      <c r="J41" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K41" s="1"/>
-      <c r="L41" s="1" t="s">
+      <c r="L41" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M41" s="1"/>
@@ -3173,15 +3055,15 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K42" s="1"/>
-      <c r="L42" s="1" t="s">
+      <c r="L42" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M42" s="1"/>
@@ -3211,7 +3093,7 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -3223,16 +3105,16 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="1" t="s">
+      <c r="J43" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K43" s="1"/>
-      <c r="L43" s="1" t="s">
+      <c r="L43" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="10" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="O43" s="6">
         <v>0.53472222222222399</v>
@@ -3257,7 +3139,7 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="11" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
@@ -3269,16 +3151,16 @@
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="1" t="s">
+      <c r="J44" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K44" s="1"/>
-      <c r="L44" s="1" t="s">
+      <c r="L44" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="O44" s="6">
         <v>0.53819444444444597</v>
@@ -3315,16 +3197,16 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="9" t="s">
-        <v>98</v>
+      <c r="J45" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="K45" s="1"/>
-      <c r="L45" s="9" t="s">
-        <v>97</v>
+      <c r="L45" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="9" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="O45" s="6">
         <v>0.54166666666666796</v>
@@ -3343,7 +3225,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>0.54513888888888995</v>
       </c>
@@ -3361,12 +3243,12 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="10" t="s">
-        <v>10</v>
+      <c r="J46" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="K46" s="1"/>
-      <c r="L46" s="10" t="s">
-        <v>10</v>
+      <c r="L46" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="10" t="s">
@@ -3407,11 +3289,11 @@
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="10" t="s">
+      <c r="J47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K47" s="1"/>
-      <c r="L47" s="10" t="s">
+      <c r="L47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M47" s="1"/>
@@ -3453,11 +3335,11 @@
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="10" t="s">
+      <c r="J48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K48" s="1"/>
-      <c r="L48" s="10" t="s">
+      <c r="L48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M48" s="1"/>
@@ -3499,11 +3381,11 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="10" t="s">
+      <c r="J49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K49" s="1"/>
-      <c r="L49" s="10" t="s">
+      <c r="L49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M49" s="1"/>
@@ -3545,11 +3427,11 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="10" t="s">
+      <c r="J50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K50" s="1"/>
-      <c r="L50" s="10" t="s">
+      <c r="L50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M50" s="1"/>
@@ -3583,7 +3465,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -3591,12 +3473,12 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="10" t="s">
-        <v>94</v>
+      <c r="J51" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K51" s="1"/>
-      <c r="L51" s="10" t="s">
-        <v>93</v>
+      <c r="L51" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M51" s="1"/>
       <c r="N51" s="10" t="s">
@@ -3637,12 +3519,12 @@
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="11" t="s">
-        <v>92</v>
+      <c r="J52" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K52" s="1"/>
-      <c r="L52" s="11" t="s">
-        <v>92</v>
+      <c r="L52" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M52" s="1"/>
       <c r="N52" s="10" t="s">
@@ -3679,7 +3561,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="1"/>
@@ -3763,7 +3645,7 @@
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="10" t="s">
@@ -3775,16 +3657,16 @@
       </c>
       <c r="H55" s="18"/>
       <c r="I55" s="1"/>
-      <c r="J55" s="9" t="s">
-        <v>89</v>
+      <c r="J55" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K55" s="1"/>
-      <c r="L55" s="9" t="s">
-        <v>88</v>
+      <c r="L55" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="O55" s="6">
         <v>0.57638888888889095</v>
@@ -3821,16 +3703,16 @@
       </c>
       <c r="H56" s="18"/>
       <c r="I56" s="1"/>
-      <c r="J56" s="10" t="s">
+      <c r="J56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K56" s="1"/>
-      <c r="L56" s="10" t="s">
+      <c r="L56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O56" s="6">
         <v>0.57986111111111305</v>
@@ -3855,11 +3737,11 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="10" t="s">
@@ -3867,16 +3749,16 @@
       </c>
       <c r="H57" s="18"/>
       <c r="I57" s="1"/>
-      <c r="J57" s="10" t="s">
-        <v>10</v>
+      <c r="J57" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K57" s="1"/>
-      <c r="L57" s="10" t="s">
-        <v>10</v>
+      <c r="L57" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="9" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="O57" s="6">
         <v>0.58333333333333504</v>
@@ -3901,11 +3783,11 @@
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="10" t="s">
@@ -4039,11 +3921,11 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="10" t="s">
@@ -4052,11 +3934,11 @@
       <c r="H61" s="18"/>
       <c r="I61" s="1"/>
       <c r="J61" s="10" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="K61" s="1"/>
       <c r="L61" s="10" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="M61" s="1"/>
       <c r="N61" s="10" t="s">
@@ -4079,7 +3961,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>0.60069444444444697</v>
       </c>
@@ -4097,12 +3979,12 @@
       </c>
       <c r="H62" s="18"/>
       <c r="I62" s="1"/>
-      <c r="J62" s="11" t="s">
-        <v>76</v>
+      <c r="J62" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K62" s="1"/>
-      <c r="L62" s="11" t="s">
-        <v>76</v>
+      <c r="L62" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M62" s="1"/>
       <c r="N62" s="10" t="s">
@@ -4131,24 +4013,24 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="1"/>
-      <c r="J63" s="1" t="s">
-        <v>10</v>
+      <c r="J63" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="K63" s="1"/>
-      <c r="L63" s="1" t="s">
-        <v>10</v>
+      <c r="L63" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="M63" s="1"/>
       <c r="N63" s="10" t="s">
@@ -4177,24 +4059,24 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H64" s="18"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="1" t="s">
-        <v>10</v>
+      <c r="J64" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="K64" s="1"/>
-      <c r="L64" s="1" t="s">
-        <v>10</v>
+      <c r="L64" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="M64" s="1"/>
       <c r="N64" s="10" t="s">
@@ -4235,12 +4117,12 @@
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-      <c r="J65" s="9" t="s">
-        <v>70</v>
+      <c r="J65" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K65" s="1"/>
-      <c r="L65" s="9" t="s">
-        <v>69</v>
+      <c r="L65" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M65" s="1"/>
       <c r="N65" s="10" t="s">
@@ -4281,11 +4163,11 @@
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
-      <c r="J66" s="10" t="s">
+      <c r="J66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K66" s="1"/>
-      <c r="L66" s="10" t="s">
+      <c r="L66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M66" s="1"/>
@@ -4315,28 +4197,28 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="1"/>
-      <c r="J67" s="10" t="s">
-        <v>10</v>
+      <c r="J67" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="K67" s="1"/>
-      <c r="L67" s="10" t="s">
-        <v>10</v>
+      <c r="L67" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="10" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="O67" s="6">
         <v>0.61805555555555802</v>
@@ -4382,7 +4264,7 @@
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O68" s="6">
         <v>0.62152777777778001</v>
@@ -4407,11 +4289,11 @@
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="10" t="s">
@@ -4428,7 +4310,7 @@
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="9" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="O69" s="6">
         <v>0.625000000000003</v>
@@ -4453,11 +4335,11 @@
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="10" t="s">
@@ -4512,11 +4394,11 @@
       <c r="H71" s="18"/>
       <c r="I71" s="1"/>
       <c r="J71" s="10" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="10" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="M71" s="1"/>
       <c r="N71" s="10" t="s">
@@ -4557,12 +4439,12 @@
       </c>
       <c r="H72" s="18"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="11" t="s">
-        <v>57</v>
+      <c r="J72" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K72" s="1"/>
-      <c r="L72" s="11" t="s">
-        <v>57</v>
+      <c r="L72" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M72" s="1"/>
       <c r="N72" s="10" t="s">
@@ -4591,11 +4473,11 @@
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="10" t="s">
@@ -4603,12 +4485,12 @@
       </c>
       <c r="H73" s="18"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="1" t="s">
-        <v>10</v>
+      <c r="J73" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="K73" s="1"/>
-      <c r="L73" s="1" t="s">
-        <v>10</v>
+      <c r="L73" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="M73" s="1"/>
       <c r="N73" s="10" t="s">
@@ -4649,12 +4531,12 @@
       </c>
       <c r="H74" s="18"/>
       <c r="I74" s="1"/>
-      <c r="J74" s="1" t="s">
-        <v>10</v>
+      <c r="J74" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="K74" s="1"/>
-      <c r="L74" s="1" t="s">
-        <v>10</v>
+      <c r="L74" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="M74" s="1"/>
       <c r="N74" s="10" t="s">
@@ -4683,11 +4565,11 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="10" t="s">
@@ -4695,12 +4577,12 @@
       </c>
       <c r="H75" s="18"/>
       <c r="I75" s="1"/>
-      <c r="J75" s="9" t="s">
-        <v>52</v>
+      <c r="J75" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K75" s="1"/>
-      <c r="L75" s="9" t="s">
-        <v>51</v>
+      <c r="L75" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M75" s="1"/>
       <c r="N75" s="10" t="s">
@@ -4729,11 +4611,11 @@
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="10" t="s">
@@ -4741,11 +4623,11 @@
       </c>
       <c r="H76" s="18"/>
       <c r="I76" s="1"/>
-      <c r="J76" s="10" t="s">
+      <c r="J76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K76" s="1"/>
-      <c r="L76" s="10" t="s">
+      <c r="L76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M76" s="1"/>
@@ -4783,16 +4665,16 @@
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="1"/>
-      <c r="J77" s="10" t="s">
-        <v>10</v>
+      <c r="J77" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="K77" s="1"/>
-      <c r="L77" s="10" t="s">
-        <v>10</v>
+      <c r="L77" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="M77" s="1"/>
       <c r="N77" s="10" t="s">
@@ -4829,7 +4711,7 @@
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H78" s="18"/>
       <c r="I78" s="1"/>
@@ -4867,11 +4749,11 @@
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
@@ -4888,7 +4770,7 @@
       </c>
       <c r="M79" s="1"/>
       <c r="N79" s="10" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="O79" s="6">
         <v>0.65972222222222499</v>
@@ -4934,7 +4816,7 @@
       </c>
       <c r="M80" s="1"/>
       <c r="N80" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O80" s="6">
         <v>0.66319444444444697</v>
@@ -4967,20 +4849,20 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="1"/>
       <c r="J81" s="10" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="K81" s="1"/>
       <c r="L81" s="10" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="M81" s="1"/>
       <c r="N81" s="9" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="O81" s="6">
         <v>0.66666666666666996</v>
@@ -4999,7 +4881,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>0.67013888888889195</v>
       </c>
@@ -5017,12 +4899,12 @@
       </c>
       <c r="H82" s="18"/>
       <c r="I82" s="1"/>
-      <c r="J82" s="11" t="s">
-        <v>39</v>
+      <c r="J82" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K82" s="1"/>
-      <c r="L82" s="11" t="s">
-        <v>39</v>
+      <c r="L82" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M82" s="1"/>
       <c r="N82" s="10" t="s">
@@ -5063,12 +4945,12 @@
       </c>
       <c r="H83" s="18"/>
       <c r="I83" s="1"/>
-      <c r="J83" s="1" t="s">
-        <v>10</v>
+      <c r="J83" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="K83" s="1"/>
-      <c r="L83" s="1" t="s">
-        <v>10</v>
+      <c r="L83" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="M83" s="1"/>
       <c r="N83" s="10" t="s">
@@ -5109,12 +4991,12 @@
       </c>
       <c r="H84" s="18"/>
       <c r="I84" s="1"/>
-      <c r="J84" s="1" t="s">
-        <v>10</v>
+      <c r="J84" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="K84" s="1"/>
-      <c r="L84" s="1" t="s">
-        <v>10</v>
+      <c r="L84" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="M84" s="1"/>
       <c r="N84" s="10" t="s">
@@ -5143,11 +5025,11 @@
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="10" t="s">
@@ -5155,12 +5037,12 @@
       </c>
       <c r="H85" s="18"/>
       <c r="I85" s="1"/>
-      <c r="J85" s="9" t="s">
-        <v>36</v>
+      <c r="J85" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K85" s="1"/>
-      <c r="L85" s="9" t="s">
-        <v>35</v>
+      <c r="L85" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M85" s="1"/>
       <c r="N85" s="10" t="s">
@@ -5189,11 +5071,11 @@
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="10" t="s">
@@ -5201,11 +5083,11 @@
       </c>
       <c r="H86" s="18"/>
       <c r="I86" s="1"/>
-      <c r="J86" s="10" t="s">
+      <c r="J86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K86" s="1"/>
-      <c r="L86" s="10" t="s">
+      <c r="L86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M86" s="1"/>
@@ -5247,12 +5129,12 @@
       </c>
       <c r="H87" s="18"/>
       <c r="I87" s="1"/>
-      <c r="J87" s="10" t="s">
-        <v>10</v>
+      <c r="J87" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="K87" s="1"/>
-      <c r="L87" s="10" t="s">
-        <v>10</v>
+      <c r="L87" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="M87" s="1"/>
       <c r="N87" s="10" t="s">
@@ -5327,11 +5209,11 @@
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="10" t="s">
@@ -5427,20 +5309,20 @@
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H91" s="18"/>
       <c r="I91" s="1"/>
       <c r="J91" s="10" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K91" s="1"/>
       <c r="L91" s="10" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="M91" s="1"/>
       <c r="N91" s="10" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O91" s="6">
         <v>0.70138888888889195</v>
@@ -5477,12 +5359,12 @@
       </c>
       <c r="H92" s="18"/>
       <c r="I92" s="1"/>
-      <c r="J92" s="11" t="s">
-        <v>27</v>
+      <c r="J92" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K92" s="1"/>
-      <c r="L92" s="11" t="s">
-        <v>27</v>
+      <c r="L92" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M92" s="1"/>
       <c r="N92" s="11" t="s">
@@ -5523,15 +5405,17 @@
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
-      <c r="J93" s="1" t="s">
-        <v>10</v>
+      <c r="J93" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="K93" s="1"/>
-      <c r="L93" s="1" t="s">
-        <v>10</v>
+      <c r="L93" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
+      <c r="N93" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="O93" s="6">
         <v>0.70833333333333703</v>
       </c>
@@ -5549,7 +5433,7 @@
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>0.71180555555555902</v>
       </c>
@@ -5567,15 +5451,17 @@
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
-      <c r="J94" s="1" t="s">
-        <v>10</v>
+      <c r="J94" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="K94" s="1"/>
-      <c r="L94" s="1" t="s">
-        <v>10</v>
+      <c r="L94" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
+      <c r="N94" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O94" s="6">
         <v>0.71180555555555902</v>
       </c>
@@ -5606,7 +5492,9 @@
         <v>24</v>
       </c>
       <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
+      <c r="G95" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="H95" s="17"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1" t="s">
@@ -5617,7 +5505,9 @@
         <v>10</v>
       </c>
       <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
+      <c r="N95" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O95" s="6">
         <v>0.71527777777778101</v>
       </c>
@@ -5648,7 +5538,9 @@
         <v>22</v>
       </c>
       <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
+      <c r="G96" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="H96" s="18"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1" t="s">
@@ -5659,7 +5551,9 @@
         <v>10</v>
       </c>
       <c r="M96" s="1"/>
-      <c r="N96" s="1"/>
+      <c r="N96" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O96" s="6">
         <v>0.718750000000004</v>
       </c>
@@ -5695,11 +5589,17 @@
       </c>
       <c r="H97" s="18"/>
       <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
+      <c r="J97" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="K97" s="1"/>
-      <c r="L97" s="1"/>
+      <c r="L97" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="M97" s="1"/>
-      <c r="N97" s="1"/>
+      <c r="N97" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O97" s="6">
         <v>0.72222222222222598</v>
       </c>
@@ -5735,11 +5635,17 @@
       </c>
       <c r="H98" s="18"/>
       <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
+      <c r="J98" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K98" s="1"/>
-      <c r="L98" s="1"/>
+      <c r="L98" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
+      <c r="N98" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O98" s="6">
         <v>0.72569444444444797</v>
       </c>
@@ -5775,11 +5681,17 @@
       </c>
       <c r="H99" s="18"/>
       <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
+      <c r="J99" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
+      <c r="L99" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
+      <c r="N99" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O99" s="6">
         <v>0.72916666666666996</v>
       </c>
@@ -5815,11 +5727,17 @@
       </c>
       <c r="H100" s="18"/>
       <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
+      <c r="J100" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
+      <c r="L100" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
+      <c r="N100" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O100" s="6">
         <v>0.73263888888889295</v>
       </c>
@@ -5855,11 +5773,17 @@
       </c>
       <c r="H101" s="18"/>
       <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
+      <c r="J101" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
+      <c r="L101" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
+      <c r="N101" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O101" s="6">
         <v>0.73611111111111505</v>
       </c>
@@ -5894,11 +5818,17 @@
       </c>
       <c r="H102" s="18"/>
       <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
+      <c r="J102" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
+      <c r="L102" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
+      <c r="N102" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O102" s="6">
         <v>0.73958333333333703</v>
       </c>
@@ -5922,11 +5852,17 @@
       </c>
       <c r="H103" s="18"/>
       <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
+      <c r="J103" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
+      <c r="L103" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
+      <c r="N103" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="O103" s="6">
         <v>0.74305555555556002</v>
       </c>
@@ -5950,11 +5886,17 @@
       </c>
       <c r="H104" s="18"/>
       <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
+      <c r="J104" s="11" t="s">
+        <v>211</v>
+      </c>
       <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
+      <c r="L104" s="11" t="s">
+        <v>211</v>
+      </c>
       <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
+      <c r="N104" s="11" t="s">
+        <v>213</v>
+      </c>
       <c r="O104" s="6">
         <v>0.74652777777778201</v>
       </c>
@@ -5978,9 +5920,13 @@
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
+      <c r="J105" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
+      <c r="L105" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="6">
@@ -6006,9 +5952,13 @@
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="1"/>
-      <c r="J106" s="1"/>
+      <c r="J106" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K106" s="1"/>
-      <c r="L106" s="1"/>
+      <c r="L106" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="6">
@@ -6034,9 +5984,13 @@
       </c>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
-      <c r="J107" s="1"/>
+      <c r="J107" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K107" s="1"/>
-      <c r="L107" s="1"/>
+      <c r="L107" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="6">
@@ -6058,13 +6012,17 @@
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="11" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
+      <c r="J108" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K108" s="1"/>
-      <c r="L108" s="1"/>
+      <c r="L108" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="6">
@@ -6177,16 +6135,16 @@
       <c r="A113" s="6"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="B114" s="23"/>
-      <c r="C114" s="19"/>
-      <c r="N114" s="20" t="str">
+      <c r="A114" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" s="22"/>
+      <c r="C114" s="23"/>
+      <c r="N114" s="19" t="str">
         <f>A114</f>
-        <v>Last updated: 26.06.2017 14:45</v>
-      </c>
-      <c r="O114" s="21"/>
+        <v>Last updated: 27.06.2017 14:55</v>
+      </c>
+      <c r="O114" s="20"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
@@ -6323,8 +6281,8 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6340,25 +6298,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6369,13 +6327,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -6388,38 +6346,38 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>0.40277777777777773</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="B4" s="14">
-        <v>0.43055555555555558</v>
+        <v>0.4375</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>156</v>
+        <v>201</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6430,1123 +6388,1123 @@
         <v>0.4375</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>0.40972222222222227</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="B6" s="14">
-        <v>0.4375</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="C6" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="B7" s="14">
-        <v>0.4375</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="B8" s="14">
-        <v>0.4375</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>6</v>
-      </c>
       <c r="D8" s="15" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>0.43055555555555558</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="B9" s="14">
-        <v>0.45833333333333331</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>0.44444444444444442</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="B10" s="14">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
         <v>0.47222222222222227</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <v>0.44444444444444442</v>
-      </c>
       <c r="B12" s="14">
-        <v>0.4861111111111111</v>
+        <v>0.5</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <v>0.44444444444444442</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="B13" s="14">
-        <v>0.47222222222222227</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="B14" s="14">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="D15" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="B15" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B16" s="14">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>154</v>
-      </c>
       <c r="D16" s="15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>122</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>0.47916666666666669</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="B17" s="14">
-        <v>0.50694444444444442</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>155</v>
       </c>
       <c r="D17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="B18" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="B19" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B21" s="14">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="F21" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B22" s="14">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B23" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="B24" s="14">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="B25" s="14">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>172</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B18" s="14">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B19" s="14">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>0.49305555555555558</v>
-      </c>
-      <c r="B20" s="14">
-        <v>0.53472222222222221</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="B21" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="B22" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="B23" s="14">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B24" s="14">
-        <v>0.56944444444444442</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B25" s="14">
-        <v>0.56944444444444442</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>179</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <v>0.54166666666666663</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="B26" s="14">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <v>0.5625</v>
-      </c>
       <c r="B27" s="14">
-        <v>0.59027777777777779</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>155</v>
+        <v>5</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
-        <v>0.56944444444444442</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="B28" s="14">
         <v>0.61111111111111105</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>165</v>
+        <v>6</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
-        <v>0.57638888888888895</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="B29" s="14">
-        <v>0.59027777777777779</v>
+        <v>0.625</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>90</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
-        <v>0.57638888888888895</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="B30" s="14">
-        <v>0.60416666666666663</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>5</v>
+        <v>145</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
-        <v>0.57638888888888895</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="B31" s="14">
-        <v>0.60416666666666663</v>
+        <v>0.61111111111111105</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
-        <v>0.58333333333333337</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B32" s="14">
-        <v>0.625</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D32" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>83</v>
-      </c>
       <c r="F32" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
-        <v>0.59722222222222221</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B33" s="14">
-        <v>0.61111111111111105</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
-        <v>0.59722222222222221</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B34" s="14">
-        <v>0.61111111111111105</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>155</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
-        <v>0.61111111111111105</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B35" s="14">
-        <v>0.63888888888888895</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>59</v>
+        <v>207</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
-        <v>0.61111111111111105</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B36" s="14">
-        <v>0.63888888888888895</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
-        <v>0.61805555555555558</v>
+        <v>0.625</v>
       </c>
       <c r="B37" s="14">
-        <v>0.63194444444444442</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>154</v>
+        <v>7</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
-        <v>0.61805555555555558</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="B38" s="14">
-        <v>0.63194444444444442</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
-        <v>0.61805555555555558</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="B39" s="14">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="B40" s="14">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="B41" s="14">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
         <v>0.65972222222222221</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
-        <v>0.625</v>
-      </c>
-      <c r="B40" s="14">
+      <c r="B42" s="14">
+        <v>0.6875</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="B43" s="14">
+        <v>0.6875</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
         <v>0.66666666666666663</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="B41" s="14">
-        <v>0.65277777777777779</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="G41" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
-        <v>0.63888888888888895</v>
-      </c>
-      <c r="B42" s="14">
-        <v>0.65277777777777779</v>
-      </c>
-      <c r="C42" s="15" t="s">
+      <c r="B44" s="14">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="B43" s="14">
-        <v>0.67361111111111116</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="B44" s="14">
-        <v>0.67361111111111116</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>6</v>
-      </c>
       <c r="D44" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>51</v>
-      </c>
       <c r="F44" s="15" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="G44" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
-        <v>0.65972222222222221</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="B45" s="14">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
         <v>0.6875</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="14">
-        <v>0.65972222222222221</v>
-      </c>
       <c r="B46" s="14">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
         <v>0.6875</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="14">
-        <v>0.66666666666666663</v>
-      </c>
       <c r="B47" s="14">
-        <v>0.70833333333333337</v>
+        <v>0.71527777777777779</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>165</v>
+        <v>6</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
-        <v>0.66666666666666663</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="B48" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="B49" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="B50" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D50" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="B51" s="14">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="B52" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="B53" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="14">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="B49" s="14">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="14">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="B50" s="14">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="14">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="B51" s="14">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="14">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="B52" s="14">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="14">
-        <v>0.71527777777777779</v>
-      </c>
-      <c r="B53" s="14">
-        <v>0.75694444444444453</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>14</v>
-      </c>
       <c r="E53" s="15" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7557,7 +7515,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>19</v>
@@ -7566,10 +7524,10 @@
         <v>21</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7580,7 +7538,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>18</v>
@@ -7589,10 +7547,10 @@
         <v>20</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7603,7 +7561,7 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>13</v>
@@ -7612,10 +7570,10 @@
         <v>16</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7626,7 +7584,7 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>12</v>
@@ -7635,28 +7593,25 @@
         <v>15</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="14">
+      <c r="A58">
         <v>0.77083333333333337</v>
       </c>
-      <c r="B58" s="14">
+      <c r="B58">
         <v>0.77777777777777779</v>
       </c>
-      <c r="C58" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15" t="s">
+      <c r="C58" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Update Agenda, PDF, XLSX and Speaker Info (28.06.2017)
</commit_message>
<xml_diff>
--- a/src/downloads/ui5con_2017_agenda.xlsx
+++ b/src/downloads/ui5con_2017_agenda.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="217">
   <si>
     <r>
       <rPr>
@@ -228,15 +228,9 @@
     <t>Aparna Narayanaswamy</t>
   </si>
   <si>
-    <t>Gregor Brett</t>
-  </si>
-  <si>
     <t>Controlling UI5 Apps and FLP via Speech</t>
   </si>
   <si>
-    <t>Building a companion conversational UI for a Fiori App</t>
-  </si>
-  <si>
     <t>Vered Constantin</t>
   </si>
   <si>
@@ -621,9 +615,6 @@
     <t>Session Description: In this session I will discuss options how UI5 web apps can be used as a basis for apps beyond your typical office requirements. While SAP Fiori apps and Fiori LaunchPad are the basis for SAPs Digital Workplace of the future, there exist much more possibilities how the web can be the basis for your digitalization efforts. We are looking into WebAPIs, standards such as WebRTC and 3rd party extensions and how this can be applied in enterprise settings. Adding Cloud APIs into the mix, lots of demand for feature-rich apps can already be fulfilled leveraging the web.</t>
   </si>
   <si>
-    <t>Building a Conversational UI for the Fiori My Inbox app using API.AI. I will run through the code needed and do a live demo.</t>
-  </si>
-  <si>
     <t>Modern browsers provide Web Speech API, enabling the application of speech recognition in web applications.We have developed an application that demonstrates how this browser capability can be leveraged in the FLP as a control mechanism.</t>
   </si>
   <si>
@@ -723,10 +714,13 @@
     <t>In this session, we will demonstrate how to get started on cloud foundry. We will see how to onboard onto the platform, install the necessary tools and deploy a UI5 application which makes use of platform services to persist its data.Prerequisites:Please have Node.js installed on your laptop and your own hanatrial account ready.</t>
   </si>
   <si>
-    <t xml:space="preserve">Let's build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind. Prerequisites:   - Laptop  - an SAP CP trial account </t>
-  </si>
-  <si>
-    <t>Last updated: 27.06.2017 14:55</t>
+    <t>17:30 - 18:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind. Prerequisites:   Laptop  an SAP CP trial account </t>
+  </si>
+  <si>
+    <t>Last updated: 28.06.2017 16:20</t>
   </si>
 </sst>
 </file>
@@ -1284,9 +1278,7 @@
   </sheetPr>
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114:C114"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1379,11 +1371,11 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -1494,11 +1486,11 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -1529,11 +1521,11 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1739,11 +1731,11 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1774,11 +1766,11 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1897,15 +1889,15 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="1"/>
@@ -1918,7 +1910,7 @@
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="O17" s="6">
         <v>0.44444444444444497</v>
@@ -2002,11 +1994,11 @@
       <c r="H19" s="18"/>
       <c r="I19" s="1"/>
       <c r="J19" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="10" t="s">
@@ -2173,11 +2165,11 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="10" t="s">
@@ -2194,7 +2186,7 @@
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O23" s="6">
         <v>0.46527777777777901</v>
@@ -2219,11 +2211,11 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="10" t="s">
@@ -2240,7 +2232,7 @@
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O24" s="6">
         <v>0.468750000000001</v>
@@ -2278,15 +2270,15 @@
       <c r="H25" s="18"/>
       <c r="I25" s="1"/>
       <c r="J25" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O25" s="6">
         <v>0.47222222222222299</v>
@@ -2324,11 +2316,11 @@
       <c r="H26" s="18"/>
       <c r="I26" s="1"/>
       <c r="J26" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="10" t="s">
@@ -2357,15 +2349,15 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="1"/>
@@ -2411,7 +2403,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="1"/>
@@ -2462,11 +2454,11 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="10" t="s">
@@ -2549,7 +2541,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="1"/>
@@ -2608,7 +2600,7 @@
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="O32" s="6">
         <v>0.49652777777777901</v>
@@ -2633,11 +2625,11 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2654,7 +2646,7 @@
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O33" s="6">
         <v>0.500000000000001</v>
@@ -2679,11 +2671,11 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="10" t="s">
@@ -2738,11 +2730,11 @@
       <c r="H35" s="18"/>
       <c r="I35" s="1"/>
       <c r="J35" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="10" t="s">
@@ -2784,11 +2776,11 @@
       <c r="H36" s="18"/>
       <c r="I36" s="1"/>
       <c r="J36" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="10" t="s">
@@ -2817,11 +2809,11 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="10" t="s">
@@ -2913,7 +2905,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="10" t="s">
@@ -2922,11 +2914,11 @@
       <c r="H39" s="18"/>
       <c r="I39" s="1"/>
       <c r="J39" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="10" t="s">
@@ -2959,7 +2951,7 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="10" t="s">
@@ -3009,7 +3001,7 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="1"/>
@@ -3055,7 +3047,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="1"/>
@@ -3093,7 +3085,7 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -3114,7 +3106,7 @@
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O43" s="6">
         <v>0.53472222222222399</v>
@@ -3139,7 +3131,7 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
@@ -3160,7 +3152,7 @@
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O44" s="6">
         <v>0.53819444444444597</v>
@@ -3198,15 +3190,15 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O45" s="6">
         <v>0.54166666666666796</v>
@@ -3244,11 +3236,11 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K46" s="1"/>
       <c r="L46" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="10" t="s">
@@ -3465,7 +3457,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -3561,7 +3553,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="1"/>
@@ -3645,7 +3637,7 @@
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="10" t="s">
@@ -3666,7 +3658,7 @@
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O55" s="6">
         <v>0.57638888888889095</v>
@@ -3712,7 +3704,7 @@
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O56" s="6">
         <v>0.57986111111111305</v>
@@ -3737,11 +3729,11 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="10" t="s">
@@ -3750,15 +3742,15 @@
       <c r="H57" s="18"/>
       <c r="I57" s="1"/>
       <c r="J57" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K57" s="1"/>
       <c r="L57" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O57" s="6">
         <v>0.58333333333333504</v>
@@ -3783,11 +3775,11 @@
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="10" t="s">
@@ -3921,11 +3913,11 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="10" t="s">
@@ -4013,24 +4005,24 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="1"/>
       <c r="J63" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K63" s="1"/>
       <c r="L63" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M63" s="1"/>
       <c r="N63" s="10" t="s">
@@ -4059,24 +4051,24 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H64" s="18"/>
       <c r="I64" s="1"/>
       <c r="J64" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K64" s="1"/>
       <c r="L64" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M64" s="1"/>
       <c r="N64" s="10" t="s">
@@ -4197,28 +4189,28 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="1"/>
       <c r="J67" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K67" s="1"/>
       <c r="L67" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O67" s="6">
         <v>0.61805555555555802</v>
@@ -4264,7 +4256,7 @@
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O68" s="6">
         <v>0.62152777777778001</v>
@@ -4289,11 +4281,11 @@
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="10" t="s">
@@ -4310,7 +4302,7 @@
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O69" s="6">
         <v>0.625000000000003</v>
@@ -4335,11 +4327,11 @@
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="10" t="s">
@@ -4473,11 +4465,11 @@
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="9" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="10" t="s">
@@ -4486,11 +4478,11 @@
       <c r="H73" s="18"/>
       <c r="I73" s="1"/>
       <c r="J73" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M73" s="1"/>
       <c r="N73" s="10" t="s">
@@ -4532,11 +4524,11 @@
       <c r="H74" s="18"/>
       <c r="I74" s="1"/>
       <c r="J74" s="11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="M74" s="1"/>
       <c r="N74" s="10" t="s">
@@ -4565,7 +4557,7 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="10" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="10" t="s">
@@ -4670,11 +4662,11 @@
       <c r="H77" s="18"/>
       <c r="I77" s="1"/>
       <c r="J77" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K77" s="1"/>
       <c r="L77" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M77" s="1"/>
       <c r="N77" s="10" t="s">
@@ -4770,7 +4762,7 @@
       </c>
       <c r="M79" s="1"/>
       <c r="N79" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O79" s="6">
         <v>0.65972222222222499</v>
@@ -4862,7 +4854,7 @@
       </c>
       <c r="M81" s="1"/>
       <c r="N81" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O81" s="6">
         <v>0.66666666666666996</v>
@@ -4946,11 +4938,11 @@
       <c r="H83" s="18"/>
       <c r="I83" s="1"/>
       <c r="J83" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K83" s="1"/>
       <c r="L83" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M83" s="1"/>
       <c r="N83" s="10" t="s">
@@ -4992,11 +4984,11 @@
       <c r="H84" s="18"/>
       <c r="I84" s="1"/>
       <c r="J84" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K84" s="1"/>
       <c r="L84" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M84" s="1"/>
       <c r="N84" s="10" t="s">
@@ -5452,11 +5444,11 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K94" s="1"/>
       <c r="L94" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M94" s="1"/>
       <c r="N94" s="10" t="s">
@@ -5761,7 +5753,7 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="10" t="s">
@@ -5805,8 +5797,8 @@
       <c r="A102" s="6">
         <v>0.73958333333333703</v>
       </c>
-      <c r="C102" s="11" t="s">
-        <v>17</v>
+      <c r="C102" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="11" t="s">
@@ -5839,7 +5831,7 @@
       <c r="A103" s="6">
         <v>0.74305555555556002</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D103" s="1"/>
@@ -5873,7 +5865,7 @@
       <c r="A104" s="6">
         <v>0.74652777777778201</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D104" s="1"/>
@@ -5887,15 +5879,15 @@
       <c r="H104" s="18"/>
       <c r="I104" s="1"/>
       <c r="J104" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K104" s="1"/>
       <c r="L104" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="M104" s="1"/>
       <c r="N104" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O104" s="6">
         <v>0.74652777777778201</v>
@@ -5907,8 +5899,8 @@
       <c r="A105" s="6">
         <v>0.750000000000004</v>
       </c>
-      <c r="C105" s="9" t="s">
-        <v>16</v>
+      <c r="C105" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="9" t="s">
@@ -5935,12 +5927,12 @@
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>0.75347222222222598</v>
       </c>
-      <c r="C106" s="10" t="s">
-        <v>10</v>
+      <c r="C106" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="10" t="s">
@@ -5971,8 +5963,8 @@
       <c r="A107" s="6">
         <v>0.75694444444444897</v>
       </c>
-      <c r="C107" s="10" t="s">
-        <v>13</v>
+      <c r="C107" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="10" t="s">
@@ -6003,8 +5995,8 @@
       <c r="A108" s="6">
         <v>0.76041666666667096</v>
       </c>
-      <c r="C108" s="11" t="s">
-        <v>11</v>
+      <c r="C108" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="11" t="s">
@@ -6012,7 +6004,7 @@
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
@@ -6136,13 +6128,13 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B114" s="22"/>
       <c r="C114" s="23"/>
       <c r="N114" s="19" t="str">
         <f>A114</f>
-        <v>Last updated: 27.06.2017 14:55</v>
+        <v>Last updated: 28.06.2017 16:20</v>
       </c>
       <c r="O114" s="20"/>
     </row>
@@ -6279,10 +6271,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6298,25 +6290,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6327,13 +6319,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -6346,13 +6338,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -6365,19 +6357,19 @@
         <v>0.4375</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6388,19 +6380,19 @@
         <v>0.4375</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6411,19 +6403,19 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -6434,19 +6426,19 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -6457,19 +6449,19 @@
         <v>0.4861111111111111</v>
       </c>
       <c r="C8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6483,16 +6475,16 @@
         <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6506,16 +6498,16 @@
         <v>5</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -6529,16 +6521,16 @@
         <v>6</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6555,13 +6547,13 @@
         <v>43</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6572,19 +6564,19 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6595,19 +6587,19 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6621,16 +6613,16 @@
         <v>5</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6644,16 +6636,16 @@
         <v>6</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6664,19 +6656,19 @@
         <v>0.53472222222222221</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6690,16 +6682,16 @@
         <v>7</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6710,19 +6702,19 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6733,19 +6725,19 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6759,16 +6751,16 @@
         <v>5</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6782,16 +6774,16 @@
         <v>6</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6805,16 +6797,16 @@
         <v>7</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6825,19 +6817,19 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6848,19 +6840,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C25" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6871,19 +6863,19 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6897,16 +6889,16 @@
         <v>5</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -6920,16 +6912,16 @@
         <v>6</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6943,16 +6935,16 @@
         <v>7</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -6963,19 +6955,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -6986,19 +6978,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7009,19 +7001,19 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7032,19 +7024,19 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7055,19 +7047,19 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>47</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7081,16 +7073,16 @@
         <v>5</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7104,16 +7096,16 @@
         <v>6</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7127,16 +7119,16 @@
         <v>7</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7147,19 +7139,19 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7170,19 +7162,19 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7196,16 +7188,16 @@
         <v>5</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7219,16 +7211,16 @@
         <v>6</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7239,7 +7231,7 @@
         <v>0.6875</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>37</v>
@@ -7248,10 +7240,10 @@
         <v>45</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7262,7 +7254,7 @@
         <v>0.6875</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>36</v>
@@ -7271,10 +7263,10 @@
         <v>44</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7285,7 +7277,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>30</v>
@@ -7294,10 +7286,10 @@
         <v>41</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7314,13 +7306,13 @@
         <v>43</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7340,10 +7332,10 @@
         <v>50</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7363,10 +7355,10 @@
         <v>49</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7377,7 +7369,7 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>25</v>
@@ -7386,10 +7378,10 @@
         <v>32</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7400,7 +7392,7 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>24</v>
@@ -7409,10 +7401,10 @@
         <v>31</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7432,10 +7424,10 @@
         <v>38</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7446,7 +7438,7 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>14</v>
@@ -7455,10 +7447,10 @@
         <v>23</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7478,10 +7470,10 @@
         <v>35</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7501,10 +7493,10 @@
         <v>34</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7512,10 +7504,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="B54" s="14">
-        <v>0.74305555555555547</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>19</v>
@@ -7524,10 +7516,10 @@
         <v>21</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7538,7 +7530,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>18</v>
@@ -7547,13 +7539,13 @@
         <v>20</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
         <v>0.75</v>
       </c>
@@ -7561,57 +7553,37 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
-        <v>0.75</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="B57" s="14">
-        <v>0.76388888888888884</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>12</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D57" s="15"/>
       <c r="E57" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="G57" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="B58">
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="C58" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>